<commit_message>
Signed-off-by: Shafqat Ali <shafqat.ali@CRESTECHAD.COM>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DBS bank\Milestone2_ExecutionTestRun1\Execution Results\ExecutionTestData\New folder\2_skippedBatch1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_skipBackup\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4EAA0A-B714-46A9-8ADD-C24E639C73F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="152">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -501,7 +500,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -773,23 +772,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -825,23 +807,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1017,7 +982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -1202,11 +1167,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,14 +1179,14 @@
     <col min="1" max="1" width="17.140625" style="18"/>
     <col min="2" max="2" width="34.140625" style="18" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" style="18" customWidth="1"/>
-    <col min="4" max="6" width="17.140625" style="18"/>
-    <col min="7" max="7" width="44.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="17.140625" style="18"/>
+    <col min="4" max="5" width="17.140625" style="18"/>
+    <col min="6" max="6" width="44.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="17.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>19</v>
       </c>
@@ -1232,25 +1197,22 @@
         <v>149</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" s="17" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
@@ -1267,19 +1229,16 @@
         <v>139</v>
       </c>
       <c r="F2" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
@@ -1304,11 +1263,8 @@
       <c r="H3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>23</v>
       </c>
@@ -1319,25 +1275,22 @@
         <v>37</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>24</v>
       </c>
@@ -1362,11 +1315,8 @@
       <c r="H5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>27</v>
       </c>
@@ -1391,11 +1341,8 @@
       <c r="H6" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>28</v>
       </c>
@@ -1420,11 +1367,8 @@
       <c r="H7" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>29</v>
       </c>
@@ -1449,11 +1393,8 @@
       <c r="H8" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>30</v>
       </c>
@@ -1464,25 +1405,22 @@
         <v>3</v>
       </c>
       <c r="D9" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F9" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G9" s="14">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H9" s="14">
-        <v>9</v>
-      </c>
-      <c r="I9" s="14">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>31</v>
       </c>
@@ -1507,17 +1445,14 @@
       <c r="H10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="20" t="s">
-        <v>32</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:I2">
+  <conditionalFormatting sqref="B2:H2">
     <cfRule type="beginsWith" dxfId="1" priority="1" operator="beginsWith" text="Working">
       <formula>LEFT((B2),LEN("Working"))=("Working")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:I2">
+  <conditionalFormatting sqref="B2:H2">
     <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="Not Working">
       <formula>LEFT((B2),LEN("Not Working"))=("Not Working")</formula>
     </cfRule>
@@ -1528,7 +1463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -1893,7 +1828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A65"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
update Test Data for rerun batch Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shafqat.ali\Desktop\jaya credential batches\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shafqat.ali\Desktop\jaya credential batches\rerun batches\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capabilities" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <t>OPPO_A53_Android_10.0.0_bd07c</t>
   </si>
   <si>
-    <t>11.0.0</t>
-  </si>
-  <si>
     <t>EndPoint</t>
   </si>
   <si>
@@ -489,6 +486,9 @@
   </si>
   <si>
     <t>9.0.0</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ4Plus_Android_9.0.0_94cc6</t>
   </si>
 </sst>
 </file>
@@ -987,7 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1023,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1073,7 +1073,7 @@
         <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
@@ -1123,7 +1123,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>15</v>
@@ -1172,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,10 +1186,10 @@
         <v>19</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,10 +1197,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1219,10 +1219,10 @@
         <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -1233,10 +1233,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -1247,10 +1247,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1258,10 +1258,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1269,10 +1269,10 @@
         <v>29</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test data updation for skip batch2 Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\ExecutionTestData\SkippedRerunBatches3\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="155">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -480,6 +480,30 @@
   </si>
   <si>
     <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA72018_Android_10.0.0_ef0ba</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyNote10Plus_Android_12.0.0_513d6</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyTabA7_Android_11.0.0_6ddce</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyA32_Android_11.0.0_b62bd</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
+  </si>
+  <si>
+    <t>XIAOMI_RedmiNote8Pro_Android_10.0.0_d3e8a</t>
+  </si>
+  <si>
+    <t>XIAOMI_RedmiNote5Pro_Android_9.0.0_d098d</t>
+  </si>
+  <si>
+    <t>SAMSUNG_GalaxyJ7Pro_Android_9.0.0_a715a</t>
   </si>
 </sst>
 </file>
@@ -611,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -664,6 +688,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1160,69 +1186,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.42578125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="21" t="s">
         <v>87</v>
       </c>
+      <c r="C1" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="D1" s="20" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="21" t="s">
         <v>137</v>
       </c>
+      <c r="C2" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="D2" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="N2" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="23" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P2" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1244,31 +1341,91 @@
       <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="E4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="F4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="L4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="N4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q4" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
@@ -1290,8 +1447,38 @@
       <c r="G5" s="19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="P5" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q5" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -1313,8 +1500,38 @@
       <c r="G6" s="15" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1336,8 +1553,38 @@
       <c r="G7" s="16" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="O7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="P7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1359,8 +1606,38 @@
       <c r="G8" s="16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="O8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
@@ -1382,8 +1659,38 @@
       <c r="G9" s="18">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="18">
+        <v>7</v>
+      </c>
+      <c r="I9" s="18">
+        <v>8</v>
+      </c>
+      <c r="J9" s="18">
+        <v>9</v>
+      </c>
+      <c r="K9" s="18">
+        <v>10</v>
+      </c>
+      <c r="L9" s="18">
+        <v>11</v>
+      </c>
+      <c r="M9" s="18">
+        <v>12</v>
+      </c>
+      <c r="N9" s="18">
+        <v>13</v>
+      </c>
+      <c r="O9" s="18">
+        <v>14</v>
+      </c>
+      <c r="P9" s="18">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
@@ -1403,6 +1710,36 @@
         <v>32</v>
       </c>
       <c r="G10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="16" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1416,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:U2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1844,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
@@ -1572,7 +1909,7 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
       <c r="B3">
         <v>121212</v>
       </c>
@@ -1688,7 +2025,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B12" t="s">
@@ -1714,7 +2051,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13">
         <v>121212</v>
       </c>

</xml_diff>

<commit_message>
Test data Added for skip batch 4 Signed-off-by: Admin <Admin@CTNL0060.crestechad.com>
</commit_message>
<xml_diff>
--- a/ExecutionTestData/1/TestData.xlsx
+++ b/ExecutionTestData/1/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\ExecutionTestData\SkippedRerunBatches3\1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jai Mata Dii\DBS_Automation\ExecutionTestData\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="151">
   <si>
     <t>ApplicationActivity</t>
   </si>
@@ -476,22 +476,10 @@
     <t>12.0.0</t>
   </si>
   <si>
-    <t>SAMSUNG_GalaxyFold_Android_9.0.0_d69de</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyNote20_Android_12.0.0_2b7fa</t>
-  </si>
-  <si>
     <t>SAMSUNG_GalaxyA72018_Android_10.0.0_ef0ba</t>
   </si>
   <si>
     <t>SAMSUNG_GalaxyNote10Plus_Android_12.0.0_513d6</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyTabA7_Android_11.0.0_6ddce</t>
-  </si>
-  <si>
-    <t>SAMSUNG_GalaxyA32_Android_11.0.0_b62bd</t>
   </si>
   <si>
     <t>10.0.0</t>
@@ -1186,34 +1174,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="41.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="41.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.42578125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>19</v>
       </c>
@@ -1221,52 +1205,40 @@
         <v>87</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>145</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>99</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>146</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="K1" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="L1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="J1" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>20</v>
       </c>
@@ -1274,52 +1246,40 @@
         <v>137</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>144</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="G2" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>151</v>
+      <c r="I2" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>142</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="N2" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -1359,20 +1319,8 @@
       <c r="M3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q3" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -1380,52 +1328,40 @@
         <v>42</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
@@ -1465,20 +1401,8 @@
       <c r="M5" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="N5" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
@@ -1518,20 +1442,8 @@
       <c r="M6" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="N6" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
@@ -1571,20 +1483,8 @@
       <c r="M7" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="N7" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="O7" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q7" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
@@ -1624,20 +1524,8 @@
       <c r="M8" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="N8" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="O8" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
@@ -1677,20 +1565,8 @@
       <c r="M9" s="18">
         <v>12</v>
       </c>
-      <c r="N9" s="18">
-        <v>13</v>
-      </c>
-      <c r="O9" s="18">
-        <v>14</v>
-      </c>
-      <c r="P9" s="18">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>31</v>
       </c>
@@ -1728,18 +1604,6 @@
         <v>32</v>
       </c>
       <c r="M10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q10" s="16" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>